<commit_message>
Replication logic is taking place
</commit_message>
<xml_diff>
--- a/wwwroot/reports/DuplicateTool 74.xlsx
+++ b/wwwroot/reports/DuplicateTool 74.xlsx
@@ -68,7 +68,7 @@
     <t>2216</t>
   </si>
   <si>
-    <t>45859</t>
+    <t>21-07-2025</t>
   </si>
   <si>
     <t>11:00 AM TO 01:00 PM</t>
@@ -233,7 +233,7 @@
     <t>2217</t>
   </si>
   <si>
-    <t>45861</t>
+    <t>23-07-2025</t>
   </si>
   <si>
     <t>103002</t>
@@ -347,7 +347,7 @@
     <t>2218</t>
   </si>
   <si>
-    <t>45863</t>
+    <t>25-07-2025</t>
   </si>
   <si>
     <t>103003</t>
@@ -461,7 +461,7 @@
     <t>2219</t>
   </si>
   <si>
-    <t>45866</t>
+    <t>28-07-2025</t>
   </si>
   <si>
     <t>103004</t>
@@ -572,7 +572,7 @@
     <t>2220</t>
   </si>
   <si>
-    <t>45868</t>
+    <t>30-07-2025</t>
   </si>
   <si>
     <t>103005</t>
@@ -662,7 +662,7 @@
     <t>2221</t>
   </si>
   <si>
-    <t>45870</t>
+    <t>01-08-2025</t>
   </si>
   <si>
     <t>103006</t>
@@ -743,7 +743,7 @@
     <t>2222</t>
   </si>
   <si>
-    <t>45873</t>
+    <t>04-08-2025</t>
   </si>
   <si>
     <t>103007</t>
@@ -800,7 +800,7 @@
     <t>2223</t>
   </si>
   <si>
-    <t>45875</t>
+    <t>06-08-2025</t>
   </si>
   <si>
     <t>103009</t>
@@ -866,7 +866,7 @@
     <t>2209</t>
   </si>
   <si>
-    <t>45877</t>
+    <t>08-08-2025</t>
   </si>
   <si>
     <t>BED-205(D)</t>
@@ -943,7 +943,7 @@
     <col min="5" max="5" width="12.745315551757812" customWidth="1"/>
     <col min="6" max="6" width="9.218536376953125" customWidth="1"/>
     <col min="7" max="7" width="9.162454605102539" customWidth="1"/>
-    <col min="8" max="8" width="11.069390296936035" customWidth="1"/>
+    <col min="8" max="8" width="13.382554054260254" customWidth="1"/>
     <col min="9" max="9" width="23.803110122680664" customWidth="1"/>
     <col min="10" max="10" width="11.907477378845215" customWidth="1"/>
     <col min="11" max="11" width="13.55699348449707" customWidth="1"/>

</xml_diff>